<commit_message>
update 6/30/25 - add day of month and week of month column combination as feature
</commit_message>
<xml_diff>
--- a/max_r_model_accuracies.xlsx
+++ b/max_r_model_accuracies.xlsx
@@ -457,10 +457,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8786885245901639</v>
+        <v>0.9639344262295082</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7213114754098361</v>
+        <v>0.7540983606557377</v>
       </c>
     </row>
     <row r="3">
@@ -470,10 +470,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.8524590163934426</v>
+        <v>0.9475409836065574</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7180327868852459</v>
+        <v>0.7573770491803279</v>
       </c>
     </row>
     <row r="4">
@@ -483,10 +483,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.898360655737705</v>
+        <v>0.9606557377049181</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7311475409836066</v>
+        <v>0.7475409836065574</v>
       </c>
     </row>
     <row r="5">
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.8852459016393442</v>
+        <v>0.9573770491803278</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7278688524590164</v>
+        <v>0.7573770491803279</v>
       </c>
     </row>
     <row r="6">
@@ -509,7 +509,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.898360655737705</v>
+        <v>0.9606557377049181</v>
       </c>
       <c r="C6" t="n">
         <v>0.7311475409836066</v>

</xml_diff>

<commit_message>
6/30/2025-till 3062 S/L with day of month and week of month feature added
</commit_message>
<xml_diff>
--- a/max_r_model_accuracies.xlsx
+++ b/max_r_model_accuracies.xlsx
@@ -457,10 +457,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9639344262295082</v>
+        <v>0.9609120521172638</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7540983606557377</v>
+        <v>0.749185667752443</v>
       </c>
     </row>
     <row r="3">
@@ -470,10 +470,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9475409836065574</v>
+        <v>0.9609120521172638</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7573770491803279</v>
+        <v>0.758957654723127</v>
       </c>
     </row>
     <row r="4">
@@ -483,10 +483,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9606557377049181</v>
+        <v>0.9739413680781759</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7475409836065574</v>
+        <v>0.739413680781759</v>
       </c>
     </row>
     <row r="5">
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9573770491803278</v>
+        <v>0.9674267100977199</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7573770491803279</v>
+        <v>0.758957654723127</v>
       </c>
     </row>
     <row r="6">
@@ -509,10 +509,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9606557377049181</v>
+        <v>0.9641693811074918</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7311475409836066</v>
+        <v>0.739413680781759</v>
       </c>
     </row>
   </sheetData>

</xml_diff>